<commit_message>
Se agrega educate con 1104
</commit_message>
<xml_diff>
--- a/Resultados_Simulacro_ICFES.xlsx
+++ b/Resultados_Simulacro_ICFES.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios\rs_icfes-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios\R_IEOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1CFB82-5E8E-49AA-BC9E-69F88E3EA8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72335241-8402-427A-99DE-67170064757C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4293" uniqueCount="1035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4441" uniqueCount="1039">
   <si>
     <t>Grupo</t>
   </si>
@@ -3145,6 +3145,18 @@
   </si>
   <si>
     <t>SILGADO BARBA MARCEDIS</t>
+  </si>
+  <si>
+    <t>1013381067</t>
+  </si>
+  <si>
+    <t>1035974363</t>
+  </si>
+  <si>
+    <t>RIOS RAMIREZ SARA</t>
+  </si>
+  <si>
+    <t>ED1</t>
   </si>
 </sst>
 </file>
@@ -14847,11 +14859,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1208"/>
+  <dimension ref="A1:K1245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1043" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1200" sqref="G1200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1209" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1209" sqref="K1209:K1245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -57833,6 +57845,1301 @@
         <v>13</v>
       </c>
     </row>
+    <row r="1209" spans="1:11" ht="15" customHeight="1">
+      <c r="A1209" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1209" t="s">
+        <v>681</v>
+      </c>
+      <c r="C1209" t="s">
+        <v>682</v>
+      </c>
+      <c r="D1209">
+        <v>403.9</v>
+      </c>
+      <c r="E1209">
+        <v>92</v>
+      </c>
+      <c r="F1209">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="G1209">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="H1209">
+        <v>84</v>
+      </c>
+      <c r="I1209">
+        <v>78.2</v>
+      </c>
+      <c r="J1209" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1209" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:11" ht="15" customHeight="1">
+      <c r="A1210" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1210" t="s">
+        <v>608</v>
+      </c>
+      <c r="C1210" t="s">
+        <v>609</v>
+      </c>
+      <c r="D1210">
+        <v>402</v>
+      </c>
+      <c r="E1210">
+        <v>78</v>
+      </c>
+      <c r="F1210">
+        <v>78</v>
+      </c>
+      <c r="G1210">
+        <v>84.5</v>
+      </c>
+      <c r="H1210">
+        <v>80</v>
+      </c>
+      <c r="I1210">
+        <v>83.6</v>
+      </c>
+      <c r="J1210" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1210" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:11" ht="15" customHeight="1">
+      <c r="A1211" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1211" t="s">
+        <v>612</v>
+      </c>
+      <c r="C1211" t="s">
+        <v>613</v>
+      </c>
+      <c r="D1211">
+        <v>359.8</v>
+      </c>
+      <c r="E1211">
+        <v>78</v>
+      </c>
+      <c r="F1211">
+        <v>73.2</v>
+      </c>
+      <c r="G1211">
+        <v>69</v>
+      </c>
+      <c r="H1211">
+        <v>62</v>
+      </c>
+      <c r="I1211">
+        <v>89.1</v>
+      </c>
+      <c r="J1211" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1211" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:11" ht="15" customHeight="1">
+      <c r="A1212" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1212" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C1212" t="s">
+        <v>615</v>
+      </c>
+      <c r="D1212">
+        <v>345.2</v>
+      </c>
+      <c r="E1212">
+        <v>72</v>
+      </c>
+      <c r="F1212">
+        <v>68.3</v>
+      </c>
+      <c r="G1212">
+        <v>62.1</v>
+      </c>
+      <c r="H1212">
+        <v>72</v>
+      </c>
+      <c r="I1212">
+        <v>74.5</v>
+      </c>
+      <c r="J1212" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1212" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:11" ht="15" customHeight="1">
+      <c r="A1213" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1213" t="s">
+        <v>634</v>
+      </c>
+      <c r="C1213" t="s">
+        <v>635</v>
+      </c>
+      <c r="D1213">
+        <v>327</v>
+      </c>
+      <c r="E1213">
+        <v>46</v>
+      </c>
+      <c r="F1213">
+        <v>70.7</v>
+      </c>
+      <c r="G1213">
+        <v>67.2</v>
+      </c>
+      <c r="H1213">
+        <v>80</v>
+      </c>
+      <c r="I1213">
+        <v>58.2</v>
+      </c>
+      <c r="J1213" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1213" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:11" ht="15" customHeight="1">
+      <c r="A1214" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1214" t="s">
+        <v>620</v>
+      </c>
+      <c r="C1214" t="s">
+        <v>621</v>
+      </c>
+      <c r="D1214">
+        <v>325.89999999999998</v>
+      </c>
+      <c r="E1214">
+        <v>62</v>
+      </c>
+      <c r="F1214">
+        <v>58.5</v>
+      </c>
+      <c r="G1214">
+        <v>62.1</v>
+      </c>
+      <c r="H1214">
+        <v>72</v>
+      </c>
+      <c r="I1214">
+        <v>83.6</v>
+      </c>
+      <c r="J1214" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1214" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:11" ht="15" customHeight="1">
+      <c r="A1215" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1215" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C1215" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D1215">
+        <v>321.60000000000002</v>
+      </c>
+      <c r="E1215">
+        <v>54</v>
+      </c>
+      <c r="F1215">
+        <v>56.1</v>
+      </c>
+      <c r="G1215">
+        <v>60.3</v>
+      </c>
+      <c r="H1215">
+        <v>78</v>
+      </c>
+      <c r="I1215">
+        <v>90.9</v>
+      </c>
+      <c r="J1215" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1215" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:11" ht="15" customHeight="1">
+      <c r="A1216" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1216" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1216" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1216">
+        <v>320.7</v>
+      </c>
+      <c r="E1216">
+        <v>66</v>
+      </c>
+      <c r="F1216">
+        <v>58.5</v>
+      </c>
+      <c r="G1216">
+        <v>65.5</v>
+      </c>
+      <c r="H1216">
+        <v>60</v>
+      </c>
+      <c r="I1216">
+        <v>83.6</v>
+      </c>
+      <c r="J1216" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1216" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:11" ht="15" customHeight="1">
+      <c r="A1217" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1217" t="s">
+        <v>683</v>
+      </c>
+      <c r="C1217" t="s">
+        <v>684</v>
+      </c>
+      <c r="D1217">
+        <v>318.7</v>
+      </c>
+      <c r="E1217">
+        <v>74</v>
+      </c>
+      <c r="F1217">
+        <v>63.4</v>
+      </c>
+      <c r="G1217">
+        <v>50</v>
+      </c>
+      <c r="H1217">
+        <v>70</v>
+      </c>
+      <c r="I1217">
+        <v>56.4</v>
+      </c>
+      <c r="J1217" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1217" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:11" ht="15" customHeight="1">
+      <c r="A1218" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1218" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1218" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1218">
+        <v>314.3</v>
+      </c>
+      <c r="E1218">
+        <v>54</v>
+      </c>
+      <c r="F1218">
+        <v>63.4</v>
+      </c>
+      <c r="G1218">
+        <v>60.3</v>
+      </c>
+      <c r="H1218">
+        <v>68</v>
+      </c>
+      <c r="I1218">
+        <v>80</v>
+      </c>
+      <c r="J1218" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1218" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:11" ht="15" customHeight="1">
+      <c r="A1219" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1219" t="s">
+        <v>638</v>
+      </c>
+      <c r="C1219" t="s">
+        <v>639</v>
+      </c>
+      <c r="D1219">
+        <v>307.89999999999998</v>
+      </c>
+      <c r="E1219">
+        <v>56</v>
+      </c>
+      <c r="F1219">
+        <v>65.8</v>
+      </c>
+      <c r="G1219">
+        <v>58.6</v>
+      </c>
+      <c r="H1219">
+        <v>64</v>
+      </c>
+      <c r="I1219">
+        <v>67.3</v>
+      </c>
+      <c r="J1219" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1219" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:11" ht="15" customHeight="1">
+      <c r="A1220" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1220" t="s">
+        <v>632</v>
+      </c>
+      <c r="C1220" t="s">
+        <v>633</v>
+      </c>
+      <c r="D1220">
+        <v>307.10000000000002</v>
+      </c>
+      <c r="E1220">
+        <v>52</v>
+      </c>
+      <c r="F1220">
+        <v>68.3</v>
+      </c>
+      <c r="G1220">
+        <v>67.2</v>
+      </c>
+      <c r="H1220">
+        <v>58</v>
+      </c>
+      <c r="I1220">
+        <v>61.8</v>
+      </c>
+      <c r="J1220" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1220" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:11" ht="15" customHeight="1">
+      <c r="A1221" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>616</v>
+      </c>
+      <c r="C1221" t="s">
+        <v>617</v>
+      </c>
+      <c r="D1221">
+        <v>305.60000000000002</v>
+      </c>
+      <c r="E1221">
+        <v>66</v>
+      </c>
+      <c r="F1221">
+        <v>70.7</v>
+      </c>
+      <c r="G1221">
+        <v>44.8</v>
+      </c>
+      <c r="H1221">
+        <v>76</v>
+      </c>
+      <c r="I1221">
+        <v>21.8</v>
+      </c>
+      <c r="J1221" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1221" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:11" ht="15" customHeight="1">
+      <c r="A1222" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>662</v>
+      </c>
+      <c r="C1222" t="s">
+        <v>663</v>
+      </c>
+      <c r="D1222">
+        <v>298.5</v>
+      </c>
+      <c r="E1222">
+        <v>56</v>
+      </c>
+      <c r="F1222">
+        <v>51.2</v>
+      </c>
+      <c r="G1222">
+        <v>65.5</v>
+      </c>
+      <c r="H1222">
+        <v>72</v>
+      </c>
+      <c r="I1222">
+        <v>41.8</v>
+      </c>
+      <c r="J1222" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1222" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:11" ht="15" customHeight="1">
+      <c r="A1223" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1223" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1223">
+        <v>297.10000000000002</v>
+      </c>
+      <c r="E1223">
+        <v>64</v>
+      </c>
+      <c r="F1223">
+        <v>61</v>
+      </c>
+      <c r="G1223">
+        <v>53.5</v>
+      </c>
+      <c r="H1223">
+        <v>56</v>
+      </c>
+      <c r="I1223">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="J1223" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1223" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:11" ht="15" customHeight="1">
+      <c r="A1224" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>618</v>
+      </c>
+      <c r="C1224" t="s">
+        <v>619</v>
+      </c>
+      <c r="D1224">
+        <v>295.10000000000002</v>
+      </c>
+      <c r="E1224">
+        <v>50</v>
+      </c>
+      <c r="F1224">
+        <v>63.4</v>
+      </c>
+      <c r="G1224">
+        <v>53.5</v>
+      </c>
+      <c r="H1224">
+        <v>64</v>
+      </c>
+      <c r="I1224">
+        <v>74.5</v>
+      </c>
+      <c r="J1224" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1224" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:11" ht="15" customHeight="1">
+      <c r="A1225" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1225" t="s">
+        <v>717</v>
+      </c>
+      <c r="C1225" t="s">
+        <v>718</v>
+      </c>
+      <c r="D1225">
+        <v>291.2</v>
+      </c>
+      <c r="E1225">
+        <v>70</v>
+      </c>
+      <c r="F1225">
+        <v>46.3</v>
+      </c>
+      <c r="G1225">
+        <v>56.9</v>
+      </c>
+      <c r="H1225">
+        <v>64</v>
+      </c>
+      <c r="I1225">
+        <v>45.5</v>
+      </c>
+      <c r="J1225" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1225" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:11" ht="15" customHeight="1">
+      <c r="A1226" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1226" t="s">
+        <v>630</v>
+      </c>
+      <c r="C1226" t="s">
+        <v>631</v>
+      </c>
+      <c r="D1226">
+        <v>283.3</v>
+      </c>
+      <c r="E1226">
+        <v>58</v>
+      </c>
+      <c r="F1226">
+        <v>53.7</v>
+      </c>
+      <c r="G1226">
+        <v>44.8</v>
+      </c>
+      <c r="H1226">
+        <v>66</v>
+      </c>
+      <c r="I1226">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="J1226" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1226" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:11" ht="15" customHeight="1">
+      <c r="A1227" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1227" t="s">
+        <v>723</v>
+      </c>
+      <c r="C1227" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D1227">
+        <v>274.8</v>
+      </c>
+      <c r="E1227">
+        <v>62</v>
+      </c>
+      <c r="F1227">
+        <v>43.9</v>
+      </c>
+      <c r="G1227">
+        <v>60.3</v>
+      </c>
+      <c r="H1227">
+        <v>58</v>
+      </c>
+      <c r="I1227">
+        <v>41.8</v>
+      </c>
+      <c r="J1227" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1227" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:11" ht="15" customHeight="1">
+      <c r="A1228" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1228" t="s">
+        <v>628</v>
+      </c>
+      <c r="C1228" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1228">
+        <v>272.89999999999998</v>
+      </c>
+      <c r="E1228">
+        <v>40</v>
+      </c>
+      <c r="F1228">
+        <v>53.7</v>
+      </c>
+      <c r="G1228">
+        <v>63.8</v>
+      </c>
+      <c r="H1228">
+        <v>56</v>
+      </c>
+      <c r="I1228">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="J1228" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1228" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:11" ht="15" customHeight="1">
+      <c r="A1229" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1229" t="s">
+        <v>648</v>
+      </c>
+      <c r="C1229" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1229">
+        <v>270.8</v>
+      </c>
+      <c r="E1229">
+        <v>64</v>
+      </c>
+      <c r="F1229">
+        <v>31.7</v>
+      </c>
+      <c r="G1229">
+        <v>63.8</v>
+      </c>
+      <c r="H1229">
+        <v>54</v>
+      </c>
+      <c r="I1229">
+        <v>63.6</v>
+      </c>
+      <c r="J1229" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1229" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:11" ht="15" customHeight="1">
+      <c r="A1230" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1230" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1230" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1230">
+        <v>266.10000000000002</v>
+      </c>
+      <c r="E1230">
+        <v>58</v>
+      </c>
+      <c r="F1230">
+        <v>36.6</v>
+      </c>
+      <c r="G1230">
+        <v>60.3</v>
+      </c>
+      <c r="H1230">
+        <v>46</v>
+      </c>
+      <c r="I1230">
+        <v>89.1</v>
+      </c>
+      <c r="J1230" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1230" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:11" ht="15" customHeight="1">
+      <c r="A1231" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1231" t="s">
+        <v>713</v>
+      </c>
+      <c r="C1231" t="s">
+        <v>714</v>
+      </c>
+      <c r="D1231">
+        <v>255.5</v>
+      </c>
+      <c r="E1231">
+        <v>52</v>
+      </c>
+      <c r="F1231">
+        <v>63.4</v>
+      </c>
+      <c r="G1231">
+        <v>31</v>
+      </c>
+      <c r="H1231">
+        <v>58</v>
+      </c>
+      <c r="I1231">
+        <v>50.9</v>
+      </c>
+      <c r="J1231" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1231" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:11" ht="15" customHeight="1">
+      <c r="A1232" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1232" t="s">
+        <v>701</v>
+      </c>
+      <c r="C1232" t="s">
+        <v>702</v>
+      </c>
+      <c r="D1232">
+        <v>252.6</v>
+      </c>
+      <c r="E1232">
+        <v>52</v>
+      </c>
+      <c r="F1232">
+        <v>46.3</v>
+      </c>
+      <c r="G1232">
+        <v>43.1</v>
+      </c>
+      <c r="H1232">
+        <v>66</v>
+      </c>
+      <c r="I1232">
+        <v>34.5</v>
+      </c>
+      <c r="J1232" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1232" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:11" ht="15" customHeight="1">
+      <c r="A1233" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1233" t="s">
+        <v>658</v>
+      </c>
+      <c r="C1233" t="s">
+        <v>659</v>
+      </c>
+      <c r="D1233">
+        <v>252.4</v>
+      </c>
+      <c r="E1233">
+        <v>44</v>
+      </c>
+      <c r="F1233">
+        <v>56.1</v>
+      </c>
+      <c r="G1233">
+        <v>43.1</v>
+      </c>
+      <c r="H1233">
+        <v>64</v>
+      </c>
+      <c r="I1233">
+        <v>34.5</v>
+      </c>
+      <c r="J1233" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1233" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:11" ht="15" customHeight="1">
+      <c r="A1234" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1234" t="s">
+        <v>654</v>
+      </c>
+      <c r="C1234" t="s">
+        <v>655</v>
+      </c>
+      <c r="D1234">
+        <v>229.3</v>
+      </c>
+      <c r="E1234">
+        <v>48</v>
+      </c>
+      <c r="F1234">
+        <v>39</v>
+      </c>
+      <c r="G1234">
+        <v>37.9</v>
+      </c>
+      <c r="H1234">
+        <v>52</v>
+      </c>
+      <c r="I1234">
+        <v>65.5</v>
+      </c>
+      <c r="J1234" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1234" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:11" ht="15" customHeight="1">
+      <c r="A1235" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1235" t="s">
+        <v>693</v>
+      </c>
+      <c r="C1235" t="s">
+        <v>694</v>
+      </c>
+      <c r="D1235">
+        <v>228.8</v>
+      </c>
+      <c r="E1235">
+        <v>30</v>
+      </c>
+      <c r="F1235">
+        <v>43.9</v>
+      </c>
+      <c r="G1235">
+        <v>50</v>
+      </c>
+      <c r="H1235">
+        <v>58</v>
+      </c>
+      <c r="I1235">
+        <v>49.1</v>
+      </c>
+      <c r="J1235" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1235" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:11" ht="15" customHeight="1">
+      <c r="A1236" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1236" t="s">
+        <v>743</v>
+      </c>
+      <c r="C1236" t="s">
+        <v>744</v>
+      </c>
+      <c r="D1236">
+        <v>216.2</v>
+      </c>
+      <c r="E1236">
+        <v>28</v>
+      </c>
+      <c r="F1236">
+        <v>46.3</v>
+      </c>
+      <c r="G1236">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="H1236">
+        <v>60</v>
+      </c>
+      <c r="I1236">
+        <v>40</v>
+      </c>
+      <c r="J1236" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1236" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:11" ht="15" customHeight="1">
+      <c r="A1237" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1237" t="s">
+        <v>660</v>
+      </c>
+      <c r="C1237" t="s">
+        <v>661</v>
+      </c>
+      <c r="D1237">
+        <v>205.3</v>
+      </c>
+      <c r="E1237">
+        <v>32</v>
+      </c>
+      <c r="F1237">
+        <v>41.5</v>
+      </c>
+      <c r="G1237">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="H1237">
+        <v>46</v>
+      </c>
+      <c r="I1237">
+        <v>56.4</v>
+      </c>
+      <c r="J1237" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1237" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:11" ht="15" customHeight="1">
+      <c r="A1238" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1238" t="s">
+        <v>666</v>
+      </c>
+      <c r="C1238" t="s">
+        <v>667</v>
+      </c>
+      <c r="D1238">
+        <v>198.5</v>
+      </c>
+      <c r="E1238">
+        <v>20</v>
+      </c>
+      <c r="F1238">
+        <v>53.7</v>
+      </c>
+      <c r="G1238">
+        <v>22.4</v>
+      </c>
+      <c r="H1238">
+        <v>62</v>
+      </c>
+      <c r="I1238">
+        <v>41.8</v>
+      </c>
+      <c r="J1238" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1238" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:11" ht="15" customHeight="1">
+      <c r="A1239" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1239" t="s">
+        <v>719</v>
+      </c>
+      <c r="C1239" t="s">
+        <v>720</v>
+      </c>
+      <c r="D1239">
+        <v>193.8</v>
+      </c>
+      <c r="E1239">
+        <v>48</v>
+      </c>
+      <c r="F1239">
+        <v>53.7</v>
+      </c>
+      <c r="G1239">
+        <v>27.6</v>
+      </c>
+      <c r="H1239">
+        <v>26</v>
+      </c>
+      <c r="I1239">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="J1239" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1239" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:11" ht="15" customHeight="1">
+      <c r="A1240" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1240" t="s">
+        <v>668</v>
+      </c>
+      <c r="C1240" t="s">
+        <v>669</v>
+      </c>
+      <c r="D1240">
+        <v>183.7</v>
+      </c>
+      <c r="E1240">
+        <v>36</v>
+      </c>
+      <c r="F1240">
+        <v>21.9</v>
+      </c>
+      <c r="G1240">
+        <v>43.1</v>
+      </c>
+      <c r="H1240">
+        <v>40</v>
+      </c>
+      <c r="I1240">
+        <v>54.5</v>
+      </c>
+      <c r="J1240" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1240" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:11" ht="15" customHeight="1">
+      <c r="A1241" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1241" t="s">
+        <v>715</v>
+      </c>
+      <c r="C1241" t="s">
+        <v>716</v>
+      </c>
+      <c r="D1241">
+        <v>176</v>
+      </c>
+      <c r="E1241">
+        <v>40</v>
+      </c>
+      <c r="F1241">
+        <v>29.3</v>
+      </c>
+      <c r="G1241">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="H1241">
+        <v>38</v>
+      </c>
+      <c r="I1241">
+        <v>27.3</v>
+      </c>
+      <c r="J1241" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1241" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:11" ht="15" customHeight="1">
+      <c r="A1242" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1242" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1242" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1242">
+        <v>160.6</v>
+      </c>
+      <c r="E1242">
+        <v>40</v>
+      </c>
+      <c r="F1242">
+        <v>24.4</v>
+      </c>
+      <c r="G1242">
+        <v>34.5</v>
+      </c>
+      <c r="H1242">
+        <v>30</v>
+      </c>
+      <c r="I1242">
+        <v>30.9</v>
+      </c>
+      <c r="J1242" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1242" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:11" ht="15" customHeight="1">
+      <c r="A1243" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1243" t="s">
+        <v>687</v>
+      </c>
+      <c r="C1243" t="s">
+        <v>688</v>
+      </c>
+      <c r="D1243">
+        <v>145.9</v>
+      </c>
+      <c r="E1243">
+        <v>24</v>
+      </c>
+      <c r="F1243">
+        <v>34.1</v>
+      </c>
+      <c r="G1243">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="H1243">
+        <v>20</v>
+      </c>
+      <c r="I1243">
+        <v>36.4</v>
+      </c>
+      <c r="J1243" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1243" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:11" ht="15" customHeight="1">
+      <c r="A1244" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1244" t="s">
+        <v>676</v>
+      </c>
+      <c r="C1244" t="s">
+        <v>677</v>
+      </c>
+      <c r="D1244">
+        <v>145.69999999999999</v>
+      </c>
+      <c r="E1244">
+        <v>34</v>
+      </c>
+      <c r="F1244">
+        <v>36.6</v>
+      </c>
+      <c r="G1244">
+        <v>24.1</v>
+      </c>
+      <c r="H1244">
+        <v>20</v>
+      </c>
+      <c r="I1244">
+        <v>34.5</v>
+      </c>
+      <c r="J1244" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1244" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:11" ht="15" customHeight="1">
+      <c r="A1245" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1245" t="s">
+        <v>678</v>
+      </c>
+      <c r="C1245" t="s">
+        <v>679</v>
+      </c>
+      <c r="D1245">
+        <v>137.4</v>
+      </c>
+      <c r="E1245">
+        <v>26</v>
+      </c>
+      <c r="F1245">
+        <v>26.8</v>
+      </c>
+      <c r="G1245">
+        <v>34.5</v>
+      </c>
+      <c r="H1245">
+        <v>16</v>
+      </c>
+      <c r="I1245">
+        <v>47.3</v>
+      </c>
+      <c r="J1245" s="2">
+        <v>2025</v>
+      </c>
+      <c r="K1245" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K1064" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>